<commit_message>
Added files for LFO and unison
</commit_message>
<xml_diff>
--- a/TestPlan/Juno60_ToneTestPlan.xlsx
+++ b/TestPlan/Juno60_ToneTestPlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GitHub\Juno60\Analysis\TestPlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GitHub\Juno60\TestPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="701" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="701" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Base settings and notes" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="382">
   <si>
     <t>Base settings</t>
   </si>
@@ -389,9 +389,6 @@
     <t>Set "PWM mode" to "Manual".</t>
   </si>
   <si>
-    <t>Set the "LFO rate" to 1.</t>
-  </si>
-  <si>
     <t>Set the "LFO delay" to 0.</t>
   </si>
   <si>
@@ -887,9 +884,6 @@
     <t>Exiting Unison mode</t>
   </si>
   <si>
-    <t>4 tests</t>
-  </si>
-  <si>
     <t>27 tests</t>
   </si>
   <si>
@@ -1110,6 +1104,114 @@
   </si>
   <si>
     <t>Controllers/VoiceAllocation/Juno 60 Multinote 5.wav</t>
+  </si>
+  <si>
+    <t>LFO/PitchModulation/Juno 60 LFO 2.1 DCOmod 0.wav</t>
+  </si>
+  <si>
+    <t>LFO/PitchModulation/Juno 60 LFO 2.1 DCOmod 10.wav</t>
+  </si>
+  <si>
+    <t>LFO/PitchModulation/Juno 60 LFO 2.1 DCOmod 5.wav</t>
+  </si>
+  <si>
+    <t>LFO/Rate/Juno 60 LFO mod Rate 0.wav</t>
+  </si>
+  <si>
+    <t>LFO/Rate/Juno 60 LFO mod Rate 2.5.wav</t>
+  </si>
+  <si>
+    <t>LFO/Rate/Juno 60 LFO mod Rate 5.wav</t>
+  </si>
+  <si>
+    <t>LFO/Rate/Juno 60 LFO mod Rate 7.5.wav</t>
+  </si>
+  <si>
+    <t>LFO/Rate/Juno 60 LFO mod Rate 10.wav</t>
+  </si>
+  <si>
+    <t>Set the "LFO rate" to 1Hz (slider = 2.1).</t>
+  </si>
+  <si>
+    <t>LFO/Delay/Juno 60 LFO Delay 2.5.wav</t>
+  </si>
+  <si>
+    <t>LFO/Delay/Juno 60 LFO Delay 5.wav</t>
+  </si>
+  <si>
+    <t>LFO/Delay/Juno 60 LFO Delay 7.5.wav</t>
+  </si>
+  <si>
+    <t>LFO/Delay/Juno 60 LFO Delay 10.wav</t>
+  </si>
+  <si>
+    <t>/LFO/PulseWidthModulation/Juno 60 LFO rate=2.1 PWM man Mod 0.wav</t>
+  </si>
+  <si>
+    <t>/LFO/PulseWidthModulation/Juno 60 LFO rate=2.1 PWM man Mod 2.5.wav</t>
+  </si>
+  <si>
+    <t>/LFO/PulseWidthModulation/Juno 60 LFO rate=2.1 PWM man Mod 7.5.wav</t>
+  </si>
+  <si>
+    <t>/LFO/PulseWidthModulation/Juno 60 LFO rate=2.1 PWM man Mod 10.wav</t>
+  </si>
+  <si>
+    <t>/LFO/PulseWidthModulation/Juno 60LFO rate=2.1 PWM 5 LFO Mod 0.wav</t>
+  </si>
+  <si>
+    <t>/LFO/PulseWidthModulation/Juno 60LFO rate=2.1 PWM 5 LFO Mod 10.wav</t>
+  </si>
+  <si>
+    <t>/LFO/PulseWidthModulation/Juno 60LFO rate=2.1 PWM 5 LFO Mod 7.5.wav</t>
+  </si>
+  <si>
+    <t>/LFO/PulseWidthModulation/Juno 60LFO rate=2.1 PWM 5 LFO Mod 5.wav</t>
+  </si>
+  <si>
+    <t>/LFO/PulseWidthModulation/Juno 60LFO rate=2.1 PWM 5 LFO Mod 2.5.wav</t>
+  </si>
+  <si>
+    <t>/LFO/FilterModulation/Juno 60 Filter Freq=2.5 LFO Mod 10.wav</t>
+  </si>
+  <si>
+    <t>/LFO/FilterModulation/Juno 60 Filter Freq=5 LFO Mod 0.wav</t>
+  </si>
+  <si>
+    <t>/LFO/FilterModulation/Juno 60 Filter Freq=5 LFO Mod 10.wav</t>
+  </si>
+  <si>
+    <t>/LFO/FilterModulation/Juno 60 Filter Freq=5 LFO Mod 7.5.wav</t>
+  </si>
+  <si>
+    <t>/LFO/FilterModulation/Juno 60 Filter Freq=5 LFO Mod 5.wav</t>
+  </si>
+  <si>
+    <t>/LFO/FilterModulation/Juno 60 Filter Freq=5 LFO Mod 2.5.wav</t>
+  </si>
+  <si>
+    <t>Unison/Saw LoA.wav</t>
+  </si>
+  <si>
+    <t>Unison/Saw MidA.wav</t>
+  </si>
+  <si>
+    <t>Unison/Pulse LoA.wav</t>
+  </si>
+  <si>
+    <t>Unison/Pulse MidA.wav</t>
+  </si>
+  <si>
+    <t>Unison/MultipleNote-Step1.wav</t>
+  </si>
+  <si>
+    <t>Unison/MultipleNote-Step3.wav</t>
+  </si>
+  <si>
+    <t>Unison/MultipleNote-Step2.wav</t>
+  </si>
+  <si>
+    <t>7 tests</t>
   </si>
 </sst>
 </file>
@@ -1533,11 +1635,11 @@
     </row>
     <row r="2" spans="1:6" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" s="10"/>
       <c r="F2" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -1580,7 +1682,7 @@
         <v>73</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D10" t="s">
         <v>63</v>
@@ -1970,7 +2072,7 @@
         <v>67</v>
       </c>
       <c r="D66" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2005,7 +2107,7 @@
       </c>
       <c r="B1" s="10"/>
       <c r="F1" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2032,7 +2134,7 @@
         <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2040,7 +2142,7 @@
         <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2048,7 +2150,7 @@
         <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2061,7 +2163,7 @@
         <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2069,7 +2171,7 @@
         <v>98</v>
       </c>
       <c r="D11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2077,7 +2179,7 @@
         <v>100</v>
       </c>
       <c r="D12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2090,7 +2192,7 @@
         <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2098,7 +2200,7 @@
         <v>98</v>
       </c>
       <c r="D15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2106,7 +2208,7 @@
         <v>101</v>
       </c>
       <c r="D16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2121,7 +2223,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2132,7 +2234,7 @@
         <v>88</v>
       </c>
       <c r="D20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2143,7 +2245,7 @@
         <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2154,7 +2256,7 @@
         <v>88</v>
       </c>
       <c r="D22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2165,7 +2267,7 @@
         <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2176,12 +2278,12 @@
         <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26" s="1"/>
     </row>
@@ -2192,12 +2294,12 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2210,7 +2312,7 @@
         <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2218,7 +2320,7 @@
         <v>98</v>
       </c>
       <c r="D32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2226,7 +2328,7 @@
         <v>99</v>
       </c>
       <c r="D33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2239,7 +2341,7 @@
         <v>97</v>
       </c>
       <c r="D35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2247,7 +2349,7 @@
         <v>98</v>
       </c>
       <c r="D36" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2255,7 +2357,7 @@
         <v>100</v>
       </c>
       <c r="D37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2268,7 +2370,7 @@
         <v>97</v>
       </c>
       <c r="D39" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2276,7 +2378,7 @@
         <v>98</v>
       </c>
       <c r="D40" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2284,12 +2386,12 @@
         <v>101</v>
       </c>
       <c r="D41" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2299,17 +2401,17 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2320,7 +2422,7 @@
         <v>88</v>
       </c>
       <c r="D48" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2331,12 +2433,12 @@
         <v>88</v>
       </c>
       <c r="D49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2346,17 +2448,17 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2367,7 +2469,7 @@
         <v>88</v>
       </c>
       <c r="D56" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2378,15 +2480,15 @@
         <v>88</v>
       </c>
       <c r="D57" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G59" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2396,12 +2498,12 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2409,12 +2511,12 @@
         <v>99</v>
       </c>
       <c r="D63" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
@@ -2422,12 +2524,12 @@
         <v>99</v>
       </c>
       <c r="D65" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
@@ -2435,12 +2537,12 @@
         <v>99</v>
       </c>
       <c r="D67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
@@ -2448,12 +2550,12 @@
         <v>99</v>
       </c>
       <c r="D69" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
@@ -2461,12 +2563,12 @@
         <v>99</v>
       </c>
       <c r="D71" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
@@ -2474,12 +2576,12 @@
         <v>99</v>
       </c>
       <c r="D73" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
@@ -2490,7 +2592,7 @@
         <v>88</v>
       </c>
       <c r="D75" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
@@ -2501,7 +2603,7 @@
         <v>88</v>
       </c>
       <c r="D76" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
@@ -2512,7 +2614,7 @@
         <v>88</v>
       </c>
       <c r="D77" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2527,7 +2629,7 @@
   </sheetPr>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -2541,11 +2643,11 @@
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="10"/>
       <c r="F1" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2554,7 +2656,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="1"/>
     </row>
@@ -2567,19 +2669,19 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2588,10 +2690,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2603,7 +2705,7 @@
         <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2612,10 +2714,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2627,7 +2729,7 @@
         <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2636,10 +2738,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2651,7 +2753,7 @@
         <v>99</v>
       </c>
       <c r="D13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2660,10 +2762,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2675,19 +2777,19 @@
         <v>99</v>
       </c>
       <c r="D15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2696,15 +2798,15 @@
         <v>2</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D18" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B20" s="1"/>
     </row>
@@ -2717,19 +2819,19 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2738,10 +2840,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D25" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2750,10 +2852,10 @@
         <v>2.5</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D26" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2762,10 +2864,10 @@
         <v>5</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D27" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2774,10 +2876,10 @@
         <v>7.5</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D28" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2785,20 +2887,20 @@
         <v>10</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2806,10 +2908,10 @@
         <v>2.5</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D32" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2817,10 +2919,10 @@
         <v>5</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D33" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2828,10 +2930,10 @@
         <v>7.5</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D34" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2839,20 +2941,20 @@
         <v>10</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D35" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2861,10 +2963,10 @@
         <v>0</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D38" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2876,7 +2978,7 @@
         <v>88</v>
       </c>
       <c r="D39" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2885,10 +2987,10 @@
         <v>0</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D40" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2900,7 +3002,7 @@
         <v>88</v>
       </c>
       <c r="D41" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2912,7 +3014,7 @@
         <v>88</v>
       </c>
       <c r="D42" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2924,7 +3026,7 @@
         <v>88</v>
       </c>
       <c r="D43" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2932,10 +3034,10 @@
         <v>10</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D44" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2947,7 +3049,7 @@
         <v>88</v>
       </c>
       <c r="D45" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2956,10 +3058,10 @@
         <v>10</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D46" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -2993,7 +3095,7 @@
       </c>
       <c r="B1" s="10"/>
       <c r="F1" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3024,7 +3126,7 @@
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3035,7 +3137,7 @@
         <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3046,7 +3148,7 @@
         <v>79</v>
       </c>
       <c r="D9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3057,7 +3159,7 @@
         <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3068,7 +3170,7 @@
         <v>79</v>
       </c>
       <c r="D11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3104,7 +3206,7 @@
         <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3115,7 +3217,7 @@
         <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3126,7 +3228,7 @@
         <v>79</v>
       </c>
       <c r="D19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3137,7 +3239,7 @@
         <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3148,7 +3250,7 @@
         <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E21" t="s">
         <v>83</v>
@@ -3172,7 +3274,7 @@
         <v>79</v>
       </c>
       <c r="D24" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3183,7 +3285,7 @@
         <v>79</v>
       </c>
       <c r="D25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3194,7 +3296,7 @@
         <v>82</v>
       </c>
       <c r="D26" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E26" t="s">
         <v>84</v>
@@ -3233,7 +3335,7 @@
         <v>90</v>
       </c>
       <c r="D32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3244,7 +3346,7 @@
         <v>90</v>
       </c>
       <c r="D33" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3255,7 +3357,7 @@
         <v>90</v>
       </c>
       <c r="D34" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3266,7 +3368,7 @@
         <v>90</v>
       </c>
       <c r="D35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3277,7 +3379,7 @@
         <v>90</v>
       </c>
       <c r="D36" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E36" t="s">
         <v>89</v>
@@ -3301,7 +3403,7 @@
         <v>90</v>
       </c>
       <c r="D39" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3312,7 +3414,7 @@
         <v>90</v>
       </c>
       <c r="D40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3323,7 +3425,7 @@
         <v>90</v>
       </c>
       <c r="D41" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3344,7 +3446,7 @@
         <v>95</v>
       </c>
       <c r="D44" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E44" t="s">
         <v>62</v>
@@ -3352,7 +3454,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3362,12 +3464,12 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3377,17 +3479,17 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3398,7 +3500,7 @@
         <v>79</v>
       </c>
       <c r="D54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3409,7 +3511,7 @@
         <v>79</v>
       </c>
       <c r="D55" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3420,15 +3522,15 @@
         <v>79</v>
       </c>
       <c r="D56" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E57" t="s">
         <v>135</v>
-      </c>
-      <c r="E57" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3439,7 +3541,7 @@
         <v>79</v>
       </c>
       <c r="D58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3450,12 +3552,12 @@
         <v>79</v>
       </c>
       <c r="D59" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3465,12 +3567,12 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
@@ -3480,22 +3582,22 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
@@ -3506,7 +3608,7 @@
         <v>79</v>
       </c>
       <c r="D70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
@@ -3517,15 +3619,15 @@
         <v>79</v>
       </c>
       <c r="D71" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E72" t="s">
         <v>135</v>
-      </c>
-      <c r="E72" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
@@ -3536,7 +3638,7 @@
         <v>79</v>
       </c>
       <c r="D73" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
@@ -3547,17 +3649,17 @@
         <v>79</v>
       </c>
       <c r="D74" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
@@ -3568,7 +3670,7 @@
         <v>79</v>
       </c>
       <c r="D77" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
@@ -3579,17 +3681,17 @@
         <v>79</v>
       </c>
       <c r="D78" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
@@ -3600,7 +3702,7 @@
         <v>79</v>
       </c>
       <c r="D81" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
@@ -3611,7 +3713,7 @@
         <v>79</v>
       </c>
       <c r="D82" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3624,8 +3726,8 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3640,7 +3742,7 @@
       </c>
       <c r="B1" s="10"/>
       <c r="F1" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3649,7 +3751,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" s="1"/>
     </row>
@@ -3662,31 +3764,31 @@
     <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="8" t="s">
-        <v>107</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3697,6 +3799,9 @@
       <c r="C10" s="7" t="s">
         <v>88</v>
       </c>
+      <c r="D10" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
@@ -3706,6 +3811,9 @@
       <c r="C11" s="7" t="s">
         <v>88</v>
       </c>
+      <c r="D11" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -3715,11 +3823,14 @@
       <c r="C12" s="7" t="s">
         <v>88</v>
       </c>
+      <c r="D12" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -3732,7 +3843,9 @@
       <c r="C14" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="1" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -3742,7 +3855,9 @@
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="13"/>
+      <c r="D15" s="1" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -3752,7 +3867,9 @@
       <c r="C16" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="1" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -3762,7 +3879,9 @@
       <c r="C17" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="1" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
@@ -3772,12 +3891,14 @@
       <c r="C18" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="13"/>
+      <c r="D18" s="1" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -3788,9 +3909,11 @@
         <v>2.5</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D20" s="13"/>
+        <v>154</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -3798,9 +3921,11 @@
         <v>5</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D21" s="13"/>
+        <v>154</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -3808,9 +3933,11 @@
         <v>7.5</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D22" s="13"/>
+        <v>154</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -3818,13 +3945,15 @@
         <v>10</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D23" s="13"/>
+        <v>154</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B25" s="1"/>
     </row>
@@ -3837,40 +3966,40 @@
     <row r="27" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="8" t="s">
-        <v>107</v>
+        <v>354</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="13">
         <v>0</v>
@@ -3878,8 +4007,11 @@
       <c r="C33" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="13">
         <v>2.5</v>
@@ -3887,8 +4019,11 @@
       <c r="C34" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="13">
         <v>5</v>
@@ -3896,8 +4031,11 @@
       <c r="C35" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="13">
         <v>7.5</v>
@@ -3905,8 +4043,11 @@
       <c r="C36" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="13">
         <v>10</v>
@@ -3914,14 +4055,17 @@
       <c r="C37" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="13">
         <v>0</v>
@@ -3929,8 +4073,11 @@
       <c r="C39" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="13">
         <v>2.5</v>
@@ -3938,8 +4085,11 @@
       <c r="C40" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="13">
         <v>7.5</v>
@@ -3947,8 +4097,11 @@
       <c r="C41" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="13">
         <v>10</v>
@@ -3956,49 +4109,52 @@
       <c r="C42" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="13">
         <v>0</v>
@@ -4007,7 +4163,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="13">
         <v>2.5</v>
@@ -4016,7 +4172,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="13">
         <v>5</v>
@@ -4025,7 +4181,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="13">
         <v>7.5</v>
@@ -4034,7 +4190,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="13">
         <v>10</v>
@@ -4042,19 +4198,22 @@
       <c r="C55" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="13">
         <v>0</v>
@@ -4062,8 +4221,11 @@
       <c r="C58" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="13">
         <v>2.5</v>
@@ -4071,8 +4233,11 @@
       <c r="C59" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="13">
         <v>5</v>
@@ -4080,8 +4245,11 @@
       <c r="C60" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="13">
         <v>7.5</v>
@@ -4089,14 +4257,20 @@
       <c r="C61" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="13">
         <v>10</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>88</v>
+      </c>
+      <c r="D62" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -4130,7 +4304,7 @@
       </c>
       <c r="B1" s="10"/>
       <c r="F1" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4139,7 +4313,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B3" s="1"/>
     </row>
@@ -4152,10 +4326,10 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4164,10 +4338,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4176,10 +4350,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4188,31 +4362,31 @@
         <v>2</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B12" s="1"/>
     </row>
@@ -4225,22 +4399,22 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E16" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4249,10 +4423,10 @@
         <v>0</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D17" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4261,10 +4435,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D18" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4273,26 +4447,26 @@
         <v>2</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D19" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D21" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -4326,7 +4500,7 @@
       </c>
       <c r="B1" s="10"/>
       <c r="F1" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4335,7 +4509,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" s="1"/>
     </row>
@@ -4347,23 +4521,23 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4374,39 +4548,39 @@
         <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4417,39 +4591,39 @@
         <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D17" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4460,23 +4634,23 @@
         <v>88</v>
       </c>
       <c r="D18" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B21" s="1"/>
     </row>
@@ -4488,23 +4662,23 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D25" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -4515,39 +4689,39 @@
         <v>88</v>
       </c>
       <c r="D26" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D27" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4558,39 +4732,39 @@
         <v>88</v>
       </c>
       <c r="D31" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D35" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4601,23 +4775,23 @@
         <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B39" s="1"/>
     </row>
@@ -4636,51 +4810,51 @@
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="15" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="15" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" s="15" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="15" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -4690,27 +4864,27 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B1" s="10"/>
       <c r="F1" s="11" t="s">
-        <v>273</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4726,19 +4900,19 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4747,44 +4921,44 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -4793,7 +4967,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B16" s="1"/>
     </row>
@@ -4817,7 +4991,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B21" s="1"/>
     </row>
@@ -4830,13 +5004,13 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -4844,12 +5018,18 @@
       <c r="B25" s="15" t="s">
         <v>97</v>
       </c>
+      <c r="D25" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="15" t="s">
         <v>99</v>
       </c>
+      <c r="D26" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="27" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
@@ -4857,7 +5037,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="B28" s="1"/>
     </row>
@@ -4870,44 +5050,98 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="1" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="1" t="s">
-        <v>282</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="33" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+        <v>97</v>
+      </c>
+      <c r="D32" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
       <c r="B33" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="15" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="1" t="s">
-        <v>268</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="16"/>
+      <c r="B40" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="16"/>
+      <c r="B41" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="1" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -4939,7 +5173,7 @@
       </c>
       <c r="B1" s="10"/>
       <c r="F1" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>